<commit_message>
Actualización de GUI y archivos de exportación
</commit_message>
<xml_diff>
--- a/CorreosInstitucionales/Server/wwwroot/assets/sol_cambio_celular.xlsx
+++ b/CorreosInstitucionales/Server/wwwroot/assets/sol_cambio_celular.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\CorreosInstitucionales\CorreosInstitucionales\Server\wwwroot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612C30A0-1067-423D-9056-5AD34E180DA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26269621-A313-4C5B-BB2D-AF3EA3721747}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="ROL" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Formato-Cuentas-Inst'!$A$4:$G$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Formato-Cuentas-Inst'!$A$4:$H$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ROL QUE DESEMPEÑA (ALUMNO, DOCENTE, ADMINISTRATIVO, EGRESADO)</t>
   </si>
@@ -80,14 +80,17 @@
     <t>NÚMERO DE CELULAR ANTERIOR</t>
   </si>
   <si>
-    <t>FECHA:                          25/04/2024</t>
+    <t>CLAVE CURP</t>
+  </si>
+  <si>
+    <t>FECHA:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +106,21 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
@@ -129,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -138,21 +156,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -252,13 +255,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,31 +271,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -658,11 +665,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,45 +677,51 @@
     <col min="1" max="1" width="29.28515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="42.85546875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="28.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="44.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="42.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="E2" s="8"/>
+      <c r="G2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="11">
+        <v>45408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="81" x14ac:dyDescent="0.25">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="81" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -722,29 +735,35 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="9"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <mergeCells count="3">
-    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:D1048576 B1:D3 D4">
+  <conditionalFormatting sqref="B5:E1048576 B1:E3 D4">
     <cfRule type="duplicateValues" dxfId="2" priority="5512"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:E3 D5:E1048576 D4">
     <cfRule type="duplicateValues" dxfId="1" priority="5585"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D1048576">
+  <conditionalFormatting sqref="D5:E1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="5588"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>